<commit_message>
files edited and updated
</commit_message>
<xml_diff>
--- a/Project RTM.xlsx
+++ b/Project RTM.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="152">
   <si>
     <t>ID: 1</t>
   </si>
@@ -129,6 +129,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Aptos Narrow"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Given</t>
     </r>
     <r>
@@ -255,7 +262,7 @@
         <rFont val="Aptos Narrow"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> the user should be redirected to their account dashboard</t>
+      <t xml:space="preserve"> the user should be redirected to Planetarium home page</t>
     </r>
   </si>
   <si>
@@ -281,6 +288,15 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>user is logged into their account and navigates to the “Planets and Moons” section and no celestial bodies have been added yet,</t>
+  </si>
+  <si>
+    <t>user fails to provide required details then system should give an error message indicating the missing fields and remain on 'Add moon 'page until required field are provided.</t>
+  </si>
+  <si>
+    <t>user clicks the “Remove” button but chooses to cancel when prompted for confirmation and moon should not be removed from the system.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -289,7 +305,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Given</t>
+      <t>When</t>
     </r>
     <r>
       <rPr>
@@ -298,17 +314,23 @@
         <rFont val="Aptos Narrow"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> the user is on the login page</t>
-    </r>
-  </si>
-  <si>
-    <t>user is logged into their account and navigates to the “Planets and Moons” section and no celestial bodies have been added yet,</t>
-  </si>
-  <si>
-    <t>user fails to provide required details then system should give an error message indicating the missing fields and remain on 'Add moon 'page until required field are provided.</t>
-  </si>
-  <si>
-    <t>user clicks the “Remove” button but chooses to cancel when prompted for confirmation and moon should not be removed from the system.</t>
+      <t xml:space="preserve"> the user provides an invalid username and/or password and clicks the login button</t>
+    </r>
+  </si>
+  <si>
+    <t>user fail to provides required details and clicks the "Add" button</t>
+  </si>
+  <si>
+    <t>user clicks the “Remove” button but chooses to cancel when prompted for confirmation and planet should not be removed from sysstem.</t>
+  </si>
+  <si>
+    <t>if user selects a planet that no longer exists and attempts to add the moon then system should display an error message, “Selected planet does not exist,”</t>
+  </si>
+  <si>
+    <t>user should be redirected back to the list of moons without any changes.</t>
+  </si>
+  <si>
+    <t>when the user provides an invalid name and/or password and clicks the create button</t>
   </si>
   <si>
     <r>
@@ -319,7 +341,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>When</t>
+      <t>Then</t>
     </r>
     <r>
       <rPr>
@@ -328,119 +350,113 @@
         <rFont val="Aptos Narrow"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> the user provides an invalid username and/or password and clicks the login button</t>
-    </r>
-  </si>
-  <si>
-    <t>user fail to provides required details and clicks the "Add" button</t>
-  </si>
-  <si>
-    <t>user clicks the “Remove” button but chooses to cancel when prompted for confirmation and planet should not be removed from sysstem.</t>
-  </si>
-  <si>
-    <t>if user selects a planet that no longer exists and attempts to add the moon then system should display an error message, “Selected planet does not exist,”</t>
-  </si>
-  <si>
-    <t>user should be redirected back to the list of moons without any changes.</t>
-  </si>
-  <si>
-    <t>when the user provides an invalid name and/or password and clicks the create button</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
+      <t xml:space="preserve"> the user should be given an alert that the login credentials are incorrect And the user should remain on the login page to try again</t>
+    </r>
+  </si>
+  <si>
+    <t>system should display a message saying, “No planets or moons available at this time and user should be given the option to add a new planet or moon.</t>
+  </si>
+  <si>
+    <t>system should give an error message indicating the missing fields</t>
+  </si>
+  <si>
+    <t>user should be redirected back to the planet list without any changes.</t>
+  </si>
+  <si>
+    <t>user should be directed back to the list of planets to select a valid planet</t>
+  </si>
+  <si>
+    <t>user attempts to remove a moon that no longer exists in the system</t>
+  </si>
+  <si>
+    <t>then the user should be given an alert saying their account hasnot  been created successfully</t>
+  </si>
+  <si>
+    <t>When the number of failed attempts reaches the limit 
+Then the account should be temporarily locked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user is viewing a specific planet in the “Planets and Moons” section and clicks on the planet's name  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> user should remain on the "Add Planet" page until all required fields are provided</t>
+  </si>
+  <si>
+    <t>user attempts to remove a planet that no longer exists in the system.</t>
+  </si>
+  <si>
+    <t>system should display an error message, “This moon no longer exists,”</t>
+  </si>
+  <si>
+    <t>and the user should stay on the registration page</t>
+  </si>
+  <si>
+    <t>user should be presented with a message explaining the account lockout</t>
+  </si>
+  <si>
+    <t>system should display a list of moons associated with that planet should be able to see the details of each moon</t>
+  </si>
+  <si>
+    <t>user enters a planet name that already exists in the system</t>
+  </si>
+  <si>
+    <t>system should display an error message, “This planet no longer exists,”</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> list of moons should be refreshed to reflect the current state</t>
+  </si>
+  <si>
+    <t>system should display an alert saying, “A planet with this name already exists,</t>
+  </si>
+  <si>
+    <t>the list of planets should be refreshed to reflect the current state.</t>
+  </si>
+  <si>
+    <t>user should be able to modify the name and attempt to add the planet again</t>
+  </si>
+  <si>
+    <t>Boundary Analysis testing for username/password length</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFFFF00"/>
-        <rFont val="Aptos Narrow"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> the user should be given an alert that the login credentials are incorrect And the user should remain on the login page to try again</t>
-    </r>
-  </si>
-  <si>
-    <t>system should display a message saying, “No planets or moons available at this time and user should be given the option to add a new planet or moon.</t>
-  </si>
-  <si>
-    <t>system should give an error message indicating the missing fields</t>
-  </si>
-  <si>
-    <t>user should be redirected back to the planet list without any changes.</t>
-  </si>
-  <si>
-    <t>user should be directed back to the list of planets to select a valid planet</t>
-  </si>
-  <si>
-    <t>user attempts to remove a moon that no longer exists in the system</t>
-  </si>
-  <si>
-    <t>then the user should be given an alert saying their account hasnot  been created successfully</t>
-  </si>
-  <si>
-    <t>When the number of failed attempts reaches the limit (e.g., 5),
-Then the account should be temporarily locked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user is viewing a specific planet in the “Planets and Moons” section and clicks on the planet's name  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> user should remain on the "Add Planet" page until all required fields are provided</t>
-  </si>
-  <si>
-    <t>user attempts to remove a planet that no longer exists in the system.</t>
-  </si>
-  <si>
-    <t>system should display an error message, “This moon no longer exists,”</t>
-  </si>
-  <si>
-    <t>and the user should stay on the registration page</t>
-  </si>
-  <si>
-    <t>user should be presented with a message explaining the account lockout</t>
-  </si>
-  <si>
-    <t>system should display a list of moons associated with that planet should be able to see the details of each moon</t>
-  </si>
-  <si>
-    <t>user enters a planet name that already exists in the system</t>
-  </si>
-  <si>
-    <t>system should display an error message, “This planet no longer exists,”</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> list of moons should be refreshed to reflect the current state</t>
-  </si>
-  <si>
-    <t>system should display an alert saying, “A planet with this name already exists,</t>
-  </si>
-  <si>
-    <t>the list of planets should be refreshed to reflect the current state.</t>
-  </si>
-  <si>
-    <t>user should be able to modify the name and attempt to add the planet again</t>
-  </si>
-  <si>
-    <t>Boundary Analysis testing for username/password length</t>
-  </si>
-  <si>
+      <t>Boundary Analysis testing for password length</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <charset val="134"/>
+      </rPr>
+      <t>: Ensure the system accepts passwords with a length no more than 30 character</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> If the list of planets/moons is paginated or limited by number, check the boundary values </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ensure the system accepts planet names that fall within the allowed character limits no more than 30 character</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> If there are limits to how many planets can be deleted at once, test the boundary values (e.g., deleting 0, 1, or the maximum number of planets).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Boundary Analysis testing for password length</t>
+      <t>Boundary Analysis testing for moon name length</t>
     </r>
     <r>
       <rPr>
@@ -449,17 +465,17 @@
         <rFont val="Aptos Narrow"/>
         <charset val="134"/>
       </rPr>
-      <t>: Ensure the system accepts passwords with a length between the specified minimum (e.g., 8 characters) and maximum (e.g., 30 characters).</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> If the list of planets/moons is paginated or limited by number, check the boundary values (e.g., 0, 1, max number per page).</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ensure the system accepts planet names that fall within the allowed character limits (e.g., minimum and maximum character limits).</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> If there are limits to how many planets can be deleted at once, test the boundary values (e.g., deleting 0, 1, or the maximum number of planets).</t>
+      <t>: Ensure the system accepts moon names within the allowed character range.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> If applicable, test the boundary values for how many moons can be removed at once (e.g., deleting 0, 1, or maximum moons)</t>
+  </si>
+  <si>
+    <t>Equivalence Partition testing for the uniqueness of usernames</t>
+  </si>
+  <si>
+    <t>Equivalence Partition testing for correct vs incorrect login credentials Test valid login credentials (existing username and correct password) and invalid combinations (incorrect username, incorrect password, non-existent accounts).</t>
   </si>
   <si>
     <r>
@@ -470,7 +486,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Boundary Analysis testing for moon name length</t>
+      <t>Equivalence Partition testing for filtering</t>
     </r>
     <r>
       <rPr>
@@ -479,17 +495,14 @@
         <rFont val="Aptos Narrow"/>
         <charset val="134"/>
       </rPr>
-      <t>: Ensure the system accepts moon names within the allowed character range.</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> If applicable, test the boundary values for how many moons can be removed at once (e.g., deleting 0, 1, or maximum moons)</t>
-  </si>
-  <si>
-    <t>Equivalence Partition testing for the uniqueness of usernames</t>
-  </si>
-  <si>
-    <t>Equivalence Partition testing for correct vs incorrect login credentials Test valid login credentials (existing username and correct password) and invalid combinations (incorrect username, incorrect password, non-existent accounts).</t>
+      <t>: Test valid and invalid filter criteria (e.g., filtering by valid planet name vs invalid name) and ensure proper results are returned.</t>
+    </r>
+  </si>
+  <si>
+    <t>Test valid and invalid planet details and verify correct system responses.</t>
+  </si>
+  <si>
+    <t>Test removing a valid planet vs trying to remove a non-existent planet or an already deleted one, and ensure correct system behavior.</t>
   </si>
   <si>
     <r>
@@ -500,7 +513,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Equivalence Partition testing for filtering</t>
+      <t>Equivalence Partition testing for valid vs invalid moon details</t>
     </r>
     <r>
       <rPr>
@@ -509,14 +522,14 @@
         <rFont val="Aptos Narrow"/>
         <charset val="134"/>
       </rPr>
-      <t>: Test valid and invalid filter criteria (e.g., filtering by valid planet name vs invalid name) and ensure proper results are returned.</t>
-    </r>
-  </si>
-  <si>
-    <t>Test valid and invalid planet details (e.g., valid name, size, and coordinates vs missing or invalid fields) and verify correct system responses.</t>
-  </si>
-  <si>
-    <t>Test removing a valid planet vs trying to remove a non-existent planet or an already deleted one, and ensure correct system behavior.</t>
+      <t>: Test valid moon details (e.g., correct name, orbital radius, etc.) against missing or incorrect data.</t>
+    </r>
+  </si>
+  <si>
+    <t>Test removing a valid moon vs trying to remove a non-existent or already deleted moon.</t>
+  </si>
+  <si>
+    <t>Exploratory Testing to see if passwords are in plain text in any places we have access to in the provided software</t>
   </si>
   <si>
     <r>
@@ -527,7 +540,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Equivalence Partition testing for valid vs invalid moon details</t>
+      <t>Exploratory Testing to verify if passwords are masked during input</t>
     </r>
     <r>
       <rPr>
@@ -536,14 +549,8 @@
         <rFont val="Aptos Narrow"/>
         <charset val="134"/>
       </rPr>
-      <t>: Test valid moon details (e.g., correct name, orbital radius, etc.) against missing or incorrect data.</t>
-    </r>
-  </si>
-  <si>
-    <t>Test removing a valid moon vs trying to remove a non-existent or already deleted moon.</t>
-  </si>
-  <si>
-    <t>Exploratory Testing to see if passwords are in plain text in any places we have access to in the provided software</t>
+      <t>:                                       Check all instances where the password is input (login, reset, etc.) to ensure passwords are never visible in plain text.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -554,7 +561,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Exploratory Testing to verify if passwords are masked during input</t>
+      <t>Exploratory Testing to ensure planet and moon details are accurate</t>
     </r>
     <r>
       <rPr>
@@ -563,7 +570,7 @@
         <rFont val="Aptos Narrow"/>
         <charset val="134"/>
       </rPr>
-      <t>:                                       Check all instances where the password is input (login, reset, etc.) to ensure passwords are never visible in plain text.</t>
+      <t>: Navigate through the system and confirm the correct planet/moon data is displayed, with no missing or incorrect information.</t>
     </r>
   </si>
   <si>
@@ -575,7 +582,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Exploratory Testing to ensure planet and moon details are accurate</t>
+      <t>Check user interface behavior</t>
     </r>
     <r>
       <rPr>
@@ -584,8 +591,20 @@
         <rFont val="Aptos Narrow"/>
         <charset val="134"/>
       </rPr>
-      <t>: Navigate through the system and confirm the correct planet/moon data is displayed, with no missing or incorrect information.</t>
-    </r>
+      <t xml:space="preserve">: Verify the user interface works smoothly while adding planets </t>
+    </r>
+  </si>
+  <si>
+    <t>Check if the planet and its associated moons are completely removed from the system and the database after deletion.</t>
+  </si>
+  <si>
+    <t>Test the UI’s behavior when adding moons, ensuring that it handles all required fields and button clicks correctly.</t>
+  </si>
+  <si>
+    <t>Ensure that after removing a moon, all associated data is deleted and the moon is no longer visible in the list.</t>
+  </si>
+  <si>
+    <t>Error Guess Testing to see if the passwords are in plain text in the interface for the application a regular user would have access to</t>
   </si>
   <si>
     <r>
@@ -596,7 +615,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Check user interface behavior</t>
+      <t>Error Guess Testing for account lockout</t>
     </r>
     <r>
       <rPr>
@@ -605,76 +624,7 @@
         <rFont val="Aptos Narrow"/>
         <charset val="134"/>
       </rPr>
-      <t>: Verify the user interface works smoothly while adding planets (e.g., does the "Add" button work, are the fields interactive).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Exploratory Testing to verify deletion process</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <charset val="134"/>
-      </rPr>
-      <t>: Check if the planet and its associated moons are completely removed from the system and the database after deletion.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Exploratory Testing to verify user interface interaction</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <charset val="134"/>
-      </rPr>
-      <t>: Test the UI’s behavior when adding moons, ensuring that it handles all required fields and button clicks correctly.</t>
-    </r>
-  </si>
-  <si>
-    <t>Ensure that after removing a moon, all associated data is deleted and the moon is no longer visible in the list.</t>
-  </si>
-  <si>
-    <t>Error Guess Testing to see if the passwords are in plain text in the interface for the application a regular user would have access to</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Error Guess Testing for account lockout</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <charset val="134"/>
-      </rPr>
-      <t>:     Attempt multiple failed login attempts and ensure the account is locked after the allowed number of attempts (e.g., 5 failed attempts).</t>
+      <t xml:space="preserve">:     Attempt multiple failed login attempts and ensure the account is locked after the allowed number of attempts </t>
     </r>
   </si>
   <si>
@@ -1586,7 +1536,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1627,22 +1577,23 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2009,7 +1960,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="6"/>
@@ -2024,367 +1975,367 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="27.6" spans="1:7">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="24" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" ht="27.6" spans="1:7">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="26" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" ht="27.6" spans="1:7">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="28" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" ht="27.6" spans="1:7">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25" t="s">
+      <c r="E5" s="26"/>
+      <c r="F5" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="25"/>
+      <c r="G5" s="26"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" ht="41.4" spans="1:7">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" ht="41.4" spans="1:7">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="29" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" ht="41.4" spans="1:7">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="29" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" ht="27.6" spans="1:7">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28" t="s">
+      <c r="C10" s="29"/>
+      <c r="D10" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="29" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28" t="s">
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28" t="s">
+      <c r="E11" s="29"/>
+      <c r="F11" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="28"/>
+      <c r="G11" s="29"/>
     </row>
     <row r="12" ht="41.4" spans="1:7">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29" t="s">
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="G12" s="30" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" ht="41.4" spans="1:7">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="D13" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="29" t="s">
+      <c r="G13" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="29" t="s">
+    </row>
+    <row r="14" ht="41.4" spans="1:7">
+      <c r="A14" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="30" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" ht="41.4" spans="1:7">
-      <c r="A14" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="29" t="s">
+      <c r="C14" s="30"/>
+      <c r="D14" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29" t="s">
+      <c r="E14" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="F14" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="G14" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="G14" s="29" t="s">
+    </row>
+    <row r="15" ht="27.6" spans="1:7">
+      <c r="A15" s="30" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15" ht="27.6" spans="1:7">
-      <c r="A15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="C15" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="D15" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="E15" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="F15" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="G15" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="29" t="s">
+    </row>
+    <row r="16" ht="27.6" spans="1:7">
+      <c r="A16" s="30" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="16" ht="27.6" spans="1:7">
-      <c r="A16" s="29" t="s">
+      <c r="B16" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="C16" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="D16" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="E16" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="29" t="s">
+      <c r="F16" s="30"/>
+      <c r="G16" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29" t="s">
+    </row>
+    <row r="17" ht="27.6" spans="1:7">
+      <c r="A17" s="30" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="17" ht="27.6" spans="1:7">
-      <c r="A17" s="29" t="s">
+      <c r="B17" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="C17" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="D17" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="E17" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="F17" s="30"/>
+      <c r="G17" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29" t="s">
+    </row>
+    <row r="18" ht="27.6" spans="4:7">
+      <c r="D18" s="30" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" ht="27.6" spans="4:7">
-      <c r="D18" s="29" t="s">
+      <c r="E18" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="29" t="s">
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+    </row>
+    <row r="19" spans="4:7">
+      <c r="D19" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-    </row>
-    <row r="19" spans="4:7">
-      <c r="D19" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2399,7 +2350,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="5" outlineLevelCol="6"/>
@@ -2414,141 +2365,141 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" ht="69" spans="1:7">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="C2" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="E2" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="G2" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="20" t="s">
+    </row>
+    <row r="3" ht="82.8" spans="1:7">
+      <c r="A3" s="20" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="3" ht="82.8" spans="1:7">
-      <c r="A3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="E3" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="F3" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="G3" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G3" s="20" t="s">
+    </row>
+    <row r="4" ht="69" spans="1:7">
+      <c r="A4" s="20" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" ht="69" spans="1:7">
-      <c r="A4" s="19" t="s">
+      <c r="B4" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="D4" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="E4" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F4" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="G4" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="20" t="s">
+    </row>
+    <row r="5" ht="69" spans="1:7">
+      <c r="A5" s="20" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="5" ht="69" spans="1:7">
-      <c r="A5" s="19" t="s">
+      <c r="B5" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="D5" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="E5" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="F5" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="G5" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="G5" s="20" t="s">
+    </row>
+    <row r="6" ht="55.2" spans="1:7">
+      <c r="A6" s="20" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="6" ht="55.2" spans="1:7">
-      <c r="A6" s="19" t="s">
+      <c r="B6" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="C6" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="D6" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="E6" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="F6" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="G6" s="22" t="s">
         <v>125</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2563,7 +2514,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="6" outlineLevelCol="3"/>
@@ -2576,84 +2527,85 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" ht="27.6" spans="1:4">
       <c r="A2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>136</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="4" ht="27.6" spans="1:4">
       <c r="A4" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" ht="27.6" spans="1:4">
       <c r="A5" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>141</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>142</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="8" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="16" t="s">
+      <c r="B6" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>145</v>
-      </c>
+      <c r="C6" s="16"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>146</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2678,27 +2630,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" ht="27.6" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>